<commit_message>
opzet voor verbeteren omloopplanning
</commit_message>
<xml_diff>
--- a/omloopplanning.xlsx
+++ b/omloopplanning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys.sharepoint.com/sites/TW-or/Gedeelde documenten/or/2024-2025/Jaar 2/Project5-I - OR-deel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/175d33217359976b/Documenten/Toegepaste wiskunde/Project/Verbetering_planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="11_A404D01AC6F19B62D3FD2A456779B547A22D40E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F40C9CA8-DC71-4EBD-AE25-90669A406D56}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2018,6 +2018,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2063,7 +2064,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2366,19 +2367,19 @@
   <dimension ref="A1:K721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -26441,6 +26442,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="b766b0002d27b841048f4e26ce56a6ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19b1c955cd3d6da461c7724026070e4b" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -26655,22 +26671,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8C3BC0-E912-4338-A876-A3F97CCE5DE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31FDBBFF-4A28-443E-B59F-06115841C7D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79932DD2-5B1C-4344-9313-0CD46CBD0CED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26687,21 +26705,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31FDBBFF-4A28-443E-B59F-06115841C7D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8C3BC0-E912-4338-A876-A3F97CCE5DE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>